<commit_message>
add user id  column
</commit_message>
<xml_diff>
--- a/public/templates/user_template.xlsx
+++ b/public/templates/user_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CEED\PuestosVotacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CEED\PuestosVotacion\DeviceCheck\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E8D8B4-2009-47BB-8465-9F51368BD6E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B174BA-4A0C-41AC-82FD-4B1812F5F2FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="840" windowWidth="24240" windowHeight="13020" xr2:uid="{BCE75A3A-A2D9-424C-8EAF-87583FD6DB65}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BCE75A3A-A2D9-424C-8EAF-87583FD6DB65}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>NOMBRE</t>
   </si>
@@ -63,7 +63,28 @@
     <t>Martin Delgado</t>
   </si>
   <si>
-    <t>Margarita Bedolla</t>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Agente1</t>
+  </si>
+  <si>
+    <t>santiago@gmail.com</t>
+  </si>
+  <si>
+    <t>agente10@gmail.com</t>
+  </si>
+  <si>
+    <t>caliche@gmail.com</t>
+  </si>
+  <si>
+    <t>Carlos Peña</t>
+  </si>
+  <si>
+    <t>Santiago Martinez</t>
+  </si>
+  <si>
+    <t>Margarita Hernandez</t>
   </si>
 </sst>
 </file>
@@ -426,74 +447,147 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A7F3ACD-3F2F-4F34-A49D-8BD0A722BFF9}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.5703125" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2">
+        <v>12345678</v>
+      </c>
+      <c r="D2">
+        <v>22</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3">
+        <v>1234561</v>
+      </c>
+      <c r="D3">
+        <v>21</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4">
+        <v>1234562</v>
+      </c>
+      <c r="D4">
         <v>7</v>
       </c>
-      <c r="B2">
+      <c r="E4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
         <v>321456987</v>
       </c>
-      <c r="C2">
+      <c r="D5">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E2">
+      <c r="F5">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6">
         <v>987456321</v>
       </c>
-      <c r="C3">
-        <v>7</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="D6">
+        <v>23</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E3">
+      <c r="F6">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{B2D01D31-1141-4D13-B491-E46C81B51CE0}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{F5B37465-0CBD-4818-83CE-FE5ED0A95F18}"/>
+    <hyperlink ref="E5" r:id="rId1" xr:uid="{B2D01D31-1141-4D13-B491-E46C81B51CE0}"/>
+    <hyperlink ref="E6" r:id="rId2" xr:uid="{F5B37465-0CBD-4818-83CE-FE5ED0A95F18}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{8F51F782-C0EE-4E76-9DF5-4A238A03572C}"/>
+    <hyperlink ref="E3" r:id="rId4" xr:uid="{B9AA5246-25BE-4AAF-BB33-E2C32BD21AA2}"/>
+    <hyperlink ref="E2" r:id="rId5" xr:uid="{9A88AD26-A3F8-4024-A7B3-659413E1FFA5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>